<commit_message>
Failed test cases from Instrument model filter
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_CDS_Filter_InstrumentModel-DNBSEQ-G400.xlsx
+++ b/InputFiles/TC01_CDS_Filter_InstrumentModel-DNBSEQ-G400.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation 0707\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F745C708-B1CA-49E2-87B5-C6CAA66A7F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896757DD-23CB-4BC8-B669-3376E7EE5F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -78,19 +78,6 @@
     <t>Match (f)&lt;--(g:genomic_info)
 WHERE g.instrument_model in ['DNBSEQ-G400']
 MATCH (f)--&gt;(samp:sample)--&gt;(p:participant)--&gt;(s:study)
-WITH p, s, collect(distinct samp.sample_id) as samp
-RETURN 
-coalesce(p.participant_id,'') as `Participant ID`,
-coalesce(s.study_name, '') as `Study Name`,
-coalesce(s.phs_accession,'') as `Accession`,
-coalesce(p.gender,'') as `Gender`,
-coalesce(apoc.text.join(samp, ','), '') as `Samples`
-ORDER BY `Participant ID`LIMIT 100</t>
-  </si>
-  <si>
-    <t>Match (f)&lt;--(g:genomic_info)
-WHERE g.instrument_model in ['DNBSEQ-G400']
-MATCH (f)--&gt;(samp:sample)--&gt;(p:participant)--&gt;(s:study)
 WITH p,s,samp,COLLECT(DISTINCT samp.sample_tumor_status) as tumor
 RETURN  
  coalesce(samp.sample_id, '') as `Sample ID`,
@@ -114,6 +101,26 @@
     coalesce(samp.sample_id, '') as `Sample ID`,
     coalesce(f.file_type, '') as `File Type`
 ORDER By f.file_name LIMIT 100</t>
+  </si>
+  <si>
+    <t>MATCH (p:participant)--&gt;(s:study)
+OPTIONAL MATCH (samp:sample)--&gt;(p)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+OPTIONAL MATCH (f)&lt;--(g:genomic_info)
+WITH s, p, samp, f, g, diag
+WHERE g.instrument_model in ['DNBSEQ-G400']
+WITH p
+OPTIONAL MATCH (p)--&gt;(s:study)
+OPTIONAL MATCH (samp:sample)--&gt;(p)
+WITH s, p, apoc.coll.sort(collect(distinct samp.sample_id)) as samp
+RETURN 
+coalesce(p.participant_id,'') as `Participant ID`,
+coalesce(s.study_name, '') as `Study Name`,
+coalesce(s.phs_accession,'') as `Accession`,
+coalesce(p.gender,'') as `Gender`,
+coalesce(apoc.text.join(samp, ','), '') as `Samples`
+ORDER BY p.participant_id limit 100</t>
   </si>
 </sst>
 </file>
@@ -494,7 +501,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -529,7 +536,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -546,7 +553,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
@@ -563,7 +570,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>

</xml_diff>